<commit_message>
delivery man app initial commit
</commit_message>
<xml_diff>
--- a/design/API.xlsx
+++ b/design/API.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects workspace\Delivery_git\GoDelivery\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKS\Armando\GoDelivery\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7608" tabRatio="920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -1470,9 +1470,6 @@
     <t>client/updateclient</t>
   </si>
   <si>
-    <t>deliveryman/login</t>
-  </si>
-  <si>
     <t>deliveryman/signup</t>
   </si>
   <si>
@@ -1541,6 +1538,9 @@
   </si>
   <si>
     <t>if clientId param exists get by cliendid else get all</t>
+  </si>
+  <si>
+    <t>deliveryman/signin</t>
   </si>
 </sst>
 </file>
@@ -1917,7 +1917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1929,7 +1929,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2259,20 +2259,20 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="37.5546875" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="87.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="87.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>37</v>
       </c>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="H1" s="52"/>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>38</v>
       </c>
@@ -2305,8 +2305,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="53"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="49"/>
       <c r="B3" s="36" t="s">
         <v>50</v>
       </c>
@@ -2321,8 +2321,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="49"/>
       <c r="B4" s="7" t="s">
         <v>51</v>
       </c>
@@ -2337,8 +2337,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="49"/>
       <c r="B5" s="7" t="s">
         <v>52</v>
       </c>
@@ -2353,8 +2353,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="53"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="49"/>
       <c r="B6" s="20" t="s">
         <v>141</v>
       </c>
@@ -2365,8 +2365,8 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="53"/>
       <c r="B7" s="20" t="s">
         <v>168</v>
       </c>
@@ -2377,7 +2377,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="20" t="s">
         <v>170</v>
@@ -2389,7 +2389,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="20" t="s">
         <v>183</v>
@@ -2401,7 +2401,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="36" t="s">
         <v>198</v>
       </c>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="D10" s="38"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
         <v>39</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="D11" s="39"/>
       <c r="G11" s="4" t="s">
@@ -2428,8 +2428,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="53"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
       <c r="B12" s="7" t="s">
         <v>54</v>
       </c>
@@ -2444,8 +2444,8 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="53"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="49"/>
       <c r="B13" s="7" t="s">
         <v>55</v>
       </c>
@@ -2456,20 +2456,20 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="53"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="49"/>
       <c r="B14" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D14" s="39"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="53"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
       <c r="B15" s="20" t="s">
         <v>151</v>
       </c>
@@ -2480,8 +2480,8 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="53"/>
       <c r="B16" s="20" t="s">
         <v>163</v>
       </c>
@@ -2492,7 +2492,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="32"/>
       <c r="B17" s="20" t="s">
         <v>172</v>
@@ -2504,7 +2504,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
         <v>40</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="50"/>
       <c r="B19" s="7" t="s">
         <v>58</v>
@@ -2538,7 +2538,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="50"/>
       <c r="B20" s="7" t="s">
         <v>59</v>
@@ -2554,7 +2554,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="50"/>
       <c r="B21" s="7" t="s">
         <v>60</v>
@@ -2570,7 +2570,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="50"/>
       <c r="B22" s="7" t="s">
         <v>61</v>
@@ -2586,7 +2586,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="50"/>
       <c r="B23" s="7" t="s">
         <v>62</v>
@@ -2602,7 +2602,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="50"/>
       <c r="B24" s="7" t="s">
         <v>63</v>
@@ -2618,7 +2618,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="50"/>
       <c r="B25" s="7" t="s">
         <v>64</v>
@@ -2634,7 +2634,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="50"/>
       <c r="B26" s="7" t="s">
         <v>65</v>
@@ -2644,7 +2644,7 @@
       </c>
       <c r="D26" s="39"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="50"/>
       <c r="B27" s="7" t="s">
         <v>66</v>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="D27" s="39"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>184</v>
       </c>
@@ -2666,8 +2666,8 @@
       </c>
       <c r="D28" s="39"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="53"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="49"/>
       <c r="B29" s="20" t="s">
         <v>187</v>
       </c>
@@ -2676,17 +2676,17 @@
       </c>
       <c r="D29" s="39"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="53"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="49"/>
       <c r="B30" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>231</v>
-      </c>
       <c r="D30" s="39"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>41</v>
       </c>
@@ -2698,19 +2698,19 @@
       </c>
       <c r="D31" s="39"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="40"/>
       <c r="C33" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="37"/>
       <c r="C34" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="39"/>
       <c r="C35" t="s">
         <v>210</v>
@@ -2769,17 +2769,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -2790,7 +2790,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>35</v>
       </c>
@@ -2806,7 +2806,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>34</v>
       </c>
@@ -2820,7 +2820,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>42</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -2849,7 +2849,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
@@ -2880,19 +2880,21 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -2903,12 +2905,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2919,7 +2921,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -2933,7 +2935,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
@@ -2946,7 +2948,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>33</v>
       </c>
@@ -2962,7 +2964,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="54"/>
       <c r="B6" s="5" t="s">
         <v>80</v>
@@ -2976,7 +2978,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
@@ -2990,7 +2992,7 @@
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>43</v>
       </c>
@@ -3026,17 +3028,17 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -3047,7 +3049,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>35</v>
       </c>
@@ -3063,7 +3065,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -3077,7 +3079,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
@@ -3090,7 +3092,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>33</v>
       </c>
@@ -3106,7 +3108,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
@@ -3140,17 +3142,17 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -3161,7 +3163,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>35</v>
       </c>
@@ -3177,7 +3179,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -3191,7 +3193,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
@@ -3204,7 +3206,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>33</v>
       </c>
@@ -3220,7 +3222,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="54"/>
       <c r="B6" s="5" t="s">
         <v>80</v>
@@ -3234,7 +3236,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
@@ -3248,7 +3250,7 @@
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>43</v>
       </c>
@@ -3286,17 +3288,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -3307,12 +3309,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3323,7 +3325,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -3337,7 +3339,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
@@ -3350,7 +3352,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>33</v>
       </c>
@@ -3366,7 +3368,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
@@ -3400,17 +3402,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -3421,7 +3423,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
@@ -3437,7 +3439,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
@@ -3451,7 +3453,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -3464,7 +3466,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>33</v>
       </c>
@@ -3480,7 +3482,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="24" t="s">
         <v>44</v>
@@ -3494,7 +3496,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
@@ -3529,17 +3531,17 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -3550,7 +3552,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
@@ -3566,7 +3568,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
@@ -3580,7 +3582,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -3593,7 +3595,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>33</v>
       </c>
@@ -3609,7 +3611,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
@@ -3643,17 +3645,17 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -3664,7 +3666,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
@@ -3680,7 +3682,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
@@ -3694,7 +3696,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -3707,7 +3709,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>33</v>
       </c>
@@ -3723,7 +3725,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
@@ -3755,19 +3757,21 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -3778,7 +3782,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -3794,7 +3798,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -3808,12 +3812,12 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -3821,7 +3825,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
@@ -3837,7 +3841,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="5" t="s">
         <v>44</v>
@@ -3851,7 +3855,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -3886,17 +3890,17 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -3907,7 +3911,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -3923,7 +3927,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -3937,7 +3941,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
@@ -3950,7 +3954,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
@@ -3966,7 +3970,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -3998,21 +4002,19 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E8"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -4023,7 +4025,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>35</v>
       </c>
@@ -4039,7 +4041,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -4053,7 +4055,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
@@ -4066,7 +4068,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>33</v>
       </c>
@@ -4082,7 +4084,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="54"/>
       <c r="B6" s="5" t="s">
         <v>71</v>
@@ -4096,7 +4098,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
@@ -4110,7 +4112,7 @@
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="54"/>
       <c r="B8" s="5"/>
       <c r="C8" s="7" t="s">
@@ -4124,7 +4126,7 @@
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>43</v>
       </c>
@@ -4162,17 +4164,17 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -4183,7 +4185,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4199,7 +4201,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -4213,12 +4215,12 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -4226,7 +4228,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
@@ -4242,7 +4244,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4276,17 +4278,17 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -4297,7 +4299,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4313,7 +4315,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -4327,20 +4329,20 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
@@ -4356,7 +4358,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4390,17 +4392,17 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -4411,7 +4413,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4427,7 +4429,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -4441,7 +4443,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
@@ -4454,7 +4456,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
@@ -4470,7 +4472,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4504,17 +4506,17 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -4525,7 +4527,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4541,7 +4543,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -4555,20 +4557,20 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
@@ -4584,7 +4586,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="9" t="s">
         <v>44</v>
@@ -4598,7 +4600,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -4633,17 +4635,17 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -4654,7 +4656,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4670,7 +4672,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -4684,7 +4686,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
@@ -4697,7 +4699,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
@@ -4713,7 +4715,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4749,17 +4751,17 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -4770,7 +4772,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4786,7 +4788,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -4800,18 +4802,18 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
@@ -4827,7 +4829,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4861,17 +4863,17 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -4882,7 +4884,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4898,7 +4900,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -4912,7 +4914,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
@@ -4925,7 +4927,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="405" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
@@ -4941,7 +4943,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4975,17 +4977,17 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -4996,7 +4998,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -5012,7 +5014,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -5026,7 +5028,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
@@ -5039,7 +5041,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
@@ -5055,7 +5057,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="5" t="s">
         <v>44</v>
@@ -5069,7 +5071,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -5104,17 +5106,17 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -5125,7 +5127,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
@@ -5141,7 +5143,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
@@ -5155,18 +5157,18 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="66" t="s">
         <v>33</v>
       </c>
@@ -5182,7 +5184,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="67"/>
       <c r="B6" s="24" t="s">
         <v>190</v>
@@ -5196,7 +5198,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
@@ -5232,17 +5234,17 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -5253,7 +5255,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
@@ -5269,7 +5271,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
@@ -5283,7 +5285,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -5296,7 +5298,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>33</v>
       </c>
@@ -5312,7 +5314,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
@@ -5348,17 +5350,17 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -5369,7 +5371,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>35</v>
       </c>
@@ -5385,7 +5387,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>34</v>
       </c>
@@ -5399,7 +5401,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>42</v>
       </c>
@@ -5412,7 +5414,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -5428,7 +5430,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
@@ -5464,17 +5466,17 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -5485,12 +5487,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
@@ -5501,7 +5503,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>34</v>
       </c>
@@ -5515,7 +5517,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>42</v>
       </c>
@@ -5528,7 +5530,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
         <v>33</v>
       </c>
@@ -5544,12 +5546,12 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C6" s="50"/>
       <c r="D6" s="50"/>
@@ -5580,17 +5582,17 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -5601,7 +5603,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -5617,7 +5619,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -5631,7 +5633,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
@@ -5640,7 +5642,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="66" t="s">
         <v>33</v>
       </c>
@@ -5656,7 +5658,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="67"/>
       <c r="B6" s="5" t="s">
         <v>109</v>
@@ -5670,7 +5672,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -5706,17 +5708,17 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -5727,7 +5729,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>35</v>
       </c>
@@ -5743,7 +5745,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -5757,7 +5759,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
@@ -5770,7 +5772,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>33</v>
       </c>
@@ -5786,7 +5788,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
@@ -5822,17 +5824,17 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -5843,7 +5845,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>35</v>
       </c>
@@ -5859,7 +5861,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -5873,7 +5875,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
@@ -5886,7 +5888,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>33</v>
       </c>
@@ -5902,7 +5904,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="5" t="s">
         <v>71</v>
@@ -5913,7 +5915,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="55"/>
     </row>
-    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
@@ -5924,7 +5926,7 @@
       </c>
       <c r="E7" s="55"/>
     </row>
-    <row r="8" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="7" t="s">
@@ -5935,7 +5937,7 @@
       </c>
       <c r="E8" s="55"/>
     </row>
-    <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>43</v>
       </c>
@@ -5970,17 +5972,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -5991,7 +5993,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
@@ -6007,7 +6009,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
@@ -6021,7 +6023,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -6034,7 +6036,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>33</v>
       </c>
@@ -6050,7 +6052,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="24" t="s">
         <v>44</v>
@@ -6064,7 +6066,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
@@ -6099,17 +6101,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -6120,7 +6122,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
@@ -6136,7 +6138,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
@@ -6150,7 +6152,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -6159,7 +6161,7 @@
       <c r="D4" s="20"/>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>33</v>
       </c>
@@ -6175,7 +6177,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
@@ -6209,17 +6211,17 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -6230,7 +6232,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
@@ -6246,7 +6248,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
@@ -6260,7 +6262,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -6273,7 +6275,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>33</v>
       </c>
@@ -6289,7 +6291,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
@@ -6325,17 +6327,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="83.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="56" t="s">
         <v>68</v>
@@ -6346,7 +6348,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
@@ -6362,7 +6364,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
@@ -6376,7 +6378,7 @@
       <c r="H3" s="61"/>
       <c r="I3" s="62"/>
     </row>
-    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -6389,7 +6391,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>33</v>
       </c>
@@ -6405,7 +6407,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
add update delivery man location api
</commit_message>
<xml_diff>
--- a/design/API.xlsx
+++ b/design/API.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920" firstSheet="7" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -29,20 +29,22 @@
     <sheet name="deliveryman_05" sheetId="28" r:id="rId15"/>
     <sheet name="deliveryman_06" sheetId="29" r:id="rId16"/>
     <sheet name="deliveryman_07" sheetId="32" r:id="rId17"/>
-    <sheet name="order_01" sheetId="15" r:id="rId18"/>
-    <sheet name="order_02" sheetId="16" r:id="rId19"/>
-    <sheet name="order_03" sheetId="17" r:id="rId20"/>
-    <sheet name="order_04" sheetId="19" r:id="rId21"/>
-    <sheet name="order_05" sheetId="20" r:id="rId22"/>
-    <sheet name="order_06" sheetId="21" r:id="rId23"/>
-    <sheet name="order_07" sheetId="22" r:id="rId24"/>
-    <sheet name="order_08" sheetId="23" r:id="rId25"/>
-    <sheet name="order_09" sheetId="24" r:id="rId26"/>
-    <sheet name="order_10" sheetId="25" r:id="rId27"/>
-    <sheet name="notification_01" sheetId="35" r:id="rId28"/>
-    <sheet name="notification_02" sheetId="36" r:id="rId29"/>
-    <sheet name="notification_03" sheetId="39" r:id="rId30"/>
-    <sheet name="syslog_1" sheetId="26" r:id="rId31"/>
+    <sheet name="deliveryman_08" sheetId="40" r:id="rId18"/>
+    <sheet name="deliveryman_09" sheetId="41" r:id="rId19"/>
+    <sheet name="order_01" sheetId="15" r:id="rId20"/>
+    <sheet name="order_02" sheetId="16" r:id="rId21"/>
+    <sheet name="order_03" sheetId="17" r:id="rId22"/>
+    <sheet name="order_04" sheetId="19" r:id="rId23"/>
+    <sheet name="order_05" sheetId="20" r:id="rId24"/>
+    <sheet name="order_06" sheetId="21" r:id="rId25"/>
+    <sheet name="order_07" sheetId="22" r:id="rId26"/>
+    <sheet name="order_08" sheetId="23" r:id="rId27"/>
+    <sheet name="order_09" sheetId="24" r:id="rId28"/>
+    <sheet name="order_10" sheetId="25" r:id="rId29"/>
+    <sheet name="notification_01" sheetId="35" r:id="rId30"/>
+    <sheet name="notification_02" sheetId="36" r:id="rId31"/>
+    <sheet name="notification_03" sheetId="39" r:id="rId32"/>
+    <sheet name="syslog_1" sheetId="26" r:id="rId33"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="245">
   <si>
     <t xml:space="preserve">get order list by order status </t>
   </si>
@@ -1541,6 +1543,58 @@
   </si>
   <si>
     <t>deliveryman/signin</t>
+  </si>
+  <si>
+    <t>deliveryman_08</t>
+  </si>
+  <si>
+    <t>deliveryman/updateFcmToken</t>
+  </si>
+  <si>
+    <t>{
+    deliverymanID: int,
+    fcmToken: string
+}</t>
+  </si>
+  <si>
+    <t>{
+     deliverymanID: 12345
+     fcmToken: '12345qwer'
+}</t>
+  </si>
+  <si>
+    <t>update fcmtoken of delivery man by ID.</t>
+  </si>
+  <si>
+    <t>deliveryman_09</t>
+  </si>
+  <si>
+    <t>deliveryman/updateLocation</t>
+  </si>
+  <si>
+    <t>update location of delivery man by ID.</t>
+  </si>
+  <si>
+    <t>{
+    deliverymanID: int,
+    locationLatitude string,
+    locationLongitude: string,
+}</t>
+  </si>
+  <si>
+    <t>{
+    "deliverymanID": 1,
+    "locationLatitude": 12.3423,
+    "locationLongitude": 34.562322
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": true,
+    "code": 200,
+    "message": "update Success.",
+    "data": [ ]
+}</t>
   </si>
 </sst>
 </file>
@@ -1787,7 +1841,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1876,9 +1930,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1914,6 +1965,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2257,10 +2326,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,13 +2351,13 @@
       <c r="C1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="52"/>
+      <c r="H1" s="57"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="53" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2297,7 +2366,7 @@
       <c r="C2" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="38"/>
       <c r="G2" s="19" t="s">
         <v>113</v>
       </c>
@@ -2306,14 +2375,14 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
-      <c r="B3" s="36" t="s">
+      <c r="A3" s="54"/>
+      <c r="B3" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="36" t="s">
         <v>203</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="38"/>
       <c r="G3" s="4" t="s">
         <v>115</v>
       </c>
@@ -2322,14 +2391,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
+      <c r="A4" s="54"/>
       <c r="B4" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="38"/>
       <c r="G4" s="4" t="s">
         <v>117</v>
       </c>
@@ -2338,14 +2407,14 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="38"/>
       <c r="G5" s="4" t="s">
         <v>119</v>
       </c>
@@ -2354,64 +2423,64 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="20" t="s">
         <v>141</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" s="38"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="20" t="s">
         <v>168</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" s="38"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="20" t="s">
         <v>170</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="D8" s="39"/>
+      <c r="D8" s="38"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="20" t="s">
         <v>183</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="D9" s="39"/>
+      <c r="D9" s="38"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="D10" s="38"/>
+      <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="53" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -2420,7 +2489,7 @@
       <c r="C11" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="38"/>
       <c r="G11" s="4" t="s">
         <v>121</v>
       </c>
@@ -2429,14 +2498,14 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="38"/>
       <c r="G12" s="4" t="s">
         <v>123</v>
       </c>
@@ -2445,284 +2514,308 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="38"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="D14" s="39"/>
+      <c r="D14" s="38"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
+      <c r="A15" s="54"/>
       <c r="B15" s="20" t="s">
         <v>151</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="D15" s="39"/>
+      <c r="D15" s="38"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
+      <c r="A16" s="54"/>
       <c r="B16" s="20" t="s">
         <v>163</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="D16" s="39"/>
+      <c r="D16" s="38"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="20" t="s">
         <v>172</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="D17" s="39"/>
+      <c r="D17" s="38"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="50" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="58"/>
+      <c r="B18" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D18" s="38"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="48"/>
+      <c r="B19" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D19" s="38"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C20" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="G18" s="19" t="s">
+      <c r="D20" s="38"/>
+      <c r="G20" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H20" s="19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="7" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="55"/>
+      <c r="B21" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C21" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="39"/>
-      <c r="G19" s="4" t="s">
+      <c r="D21" s="38"/>
+      <c r="G21" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="7" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="55"/>
+      <c r="B22" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="39"/>
-      <c r="G20" s="4" t="s">
+      <c r="D22" s="38"/>
+      <c r="G22" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="7" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="55"/>
+      <c r="B23" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="39"/>
-      <c r="G21" s="4" t="s">
+      <c r="D23" s="38"/>
+      <c r="G23" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="7" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="55"/>
+      <c r="B24" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C24" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="G22" s="4" t="s">
+      <c r="D24" s="38"/>
+      <c r="G24" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="7" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="55"/>
+      <c r="B25" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C25" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="39"/>
-      <c r="G23" s="4" t="s">
+      <c r="D25" s="38"/>
+      <c r="G25" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="7" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="55"/>
+      <c r="B26" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C26" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="39"/>
-      <c r="G24" s="4" t="s">
+      <c r="D26" s="38"/>
+      <c r="G26" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="7" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="55"/>
+      <c r="B27" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C27" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="39"/>
-      <c r="G25" s="4" t="s">
+      <c r="D27" s="38"/>
+      <c r="G27" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="7" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="55"/>
+      <c r="B28" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C28" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="39"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
-      <c r="B27" s="7" t="s">
+      <c r="D28" s="38"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="55"/>
+      <c r="B29" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C29" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="39"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+      <c r="D29" s="38"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B30" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C30" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="D28" s="39"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="20" t="s">
+      <c r="D30" s="38"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="54"/>
+      <c r="B31" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C31" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="D29" s="39"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="41" t="s">
+      <c r="D31" s="38"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
+      <c r="B32" s="40" t="s">
         <v>229</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C32" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="D30" s="39"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="D32" s="38"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C33" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="39"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="40"/>
-      <c r="C33" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="37"/>
-      <c r="C34" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="38"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="39"/>
       <c r="C35" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="36"/>
+      <c r="C36" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="38"/>
+      <c r="C37" t="s">
         <v>210</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A20:A29"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A11:A16"/>
     <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A11:A18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" location="client_01!A1" display="client/get"/>
@@ -2732,17 +2825,17 @@
     <hyperlink ref="C12" location="deliveryman_02!A1" display="deliveryman/totalcount"/>
     <hyperlink ref="C13" location="deliveryman_03!A1" display="deliveryman/list"/>
     <hyperlink ref="C14" location="deliveryman_04!A1" display="deliveryman/save"/>
-    <hyperlink ref="C18" location="order_01!A1" display="order/create"/>
-    <hyperlink ref="C19" location="order_02!A1" display="order/send"/>
-    <hyperlink ref="C20" location="order_03!A1" display="order/cancel"/>
-    <hyperlink ref="C21" location="order_04!A1" display="order/receive"/>
-    <hyperlink ref="C22" location="order_05!A1" display="order/rate"/>
-    <hyperlink ref="C23" location="order_06!A1" display="order/acceptrequest"/>
-    <hyperlink ref="C24" location="order_07!A1" display="orders/totalcount"/>
-    <hyperlink ref="C25" location="order_08!A1" display="order/totalearning"/>
-    <hyperlink ref="C26" location="order_09!A1" display="order/dailycount"/>
-    <hyperlink ref="C27" location="order_10!A1" display="order/list"/>
-    <hyperlink ref="C31" location="syslog_1!A1" display="syslog/list"/>
+    <hyperlink ref="C20" location="order_01!A1" display="order/create"/>
+    <hyperlink ref="C21" location="order_02!A1" display="order/send"/>
+    <hyperlink ref="C22" location="order_03!A1" display="order/cancel"/>
+    <hyperlink ref="C23" location="order_04!A1" display="order/receive"/>
+    <hyperlink ref="C24" location="order_05!A1" display="order/rate"/>
+    <hyperlink ref="C25" location="order_06!A1" display="order/acceptrequest"/>
+    <hyperlink ref="C26" location="order_07!A1" display="orders/totalcount"/>
+    <hyperlink ref="C27" location="order_08!A1" display="order/totalearning"/>
+    <hyperlink ref="C28" location="order_09!A1" display="order/dailycount"/>
+    <hyperlink ref="C29" location="order_10!A1" display="order/list"/>
+    <hyperlink ref="C33" location="syslog_1!A1" display="syslog/list"/>
     <hyperlink ref="C6" location="client_05!A1" display="client/orderlist"/>
     <hyperlink ref="C15" location="deliveryman_05!A1" display="deliveryman/orderlist"/>
     <hyperlink ref="C16" location="deliveryman_06!A1" display="deliveryman/changeState"/>
@@ -2750,10 +2843,11 @@
     <hyperlink ref="C17" location="deliveryman_07!A1" display="deliveryman/delete"/>
     <hyperlink ref="C8" location="client_07!A1" display="client/delete"/>
     <hyperlink ref="C9" location="client_08!A1" display="client/update"/>
-    <hyperlink ref="C29" location="notification_02!A1" display="notification/delete"/>
-    <hyperlink ref="C28" location="notification_01!A1" display="notification/list"/>
+    <hyperlink ref="C31" location="notification_02!A1" display="notification/delete"/>
+    <hyperlink ref="C30" location="notification_01!A1" display="notification/list"/>
     <hyperlink ref="C10" location="client_09!A1" display="client/phonecheck"/>
-    <hyperlink ref="C30" location="notification_03!A1" display="notification/create"/>
+    <hyperlink ref="C32" location="notification_03!A1" display="notification/create"/>
+    <hyperlink ref="C18" location="deliveryman_08!A1" display="deliveryman/updateFcmToken"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2781,11 +2875,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="30" t="s">
         <v>47</v>
       </c>
@@ -2800,11 +2894,11 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -2816,9 +2910,9 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
@@ -2853,12 +2947,12 @@
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2880,7 +2974,7 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2896,11 +2990,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -2915,11 +3009,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -2931,9 +3025,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -2949,7 +3043,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -2957,7 +3051,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="60" t="s">
         <v>82</v>
       </c>
       <c r="H5" s="3"/>
@@ -2965,7 +3059,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="5" t="s">
         <v>80</v>
       </c>
@@ -2973,13 +3067,13 @@
         <v>81</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="55"/>
+      <c r="E6" s="60"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -2987,7 +3081,7 @@
       <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="55"/>
+      <c r="E7" s="60"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -2996,12 +3090,12 @@
       <c r="A8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3040,11 +3134,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3059,11 +3153,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3075,9 +3169,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3112,12 +3206,12 @@
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3154,11 +3248,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3173,11 +3267,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3189,9 +3283,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3207,7 +3301,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3215,7 +3309,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="60" t="s">
         <v>82</v>
       </c>
       <c r="H5" s="3"/>
@@ -3223,7 +3317,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="5" t="s">
         <v>80</v>
       </c>
@@ -3231,13 +3325,13 @@
         <v>89</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="55"/>
+      <c r="E6" s="60"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -3245,7 +3339,7 @@
       <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="55"/>
+      <c r="E7" s="60"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -3254,12 +3348,12 @@
       <c r="A8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3300,11 +3394,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3319,11 +3413,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3335,9 +3429,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3372,12 +3466,12 @@
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3414,11 +3508,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3433,11 +3527,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3449,9 +3543,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -3475,7 +3569,7 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="68" t="s">
         <v>148</v>
       </c>
       <c r="H5" s="3"/>
@@ -3491,7 +3585,7 @@
         <v>147</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="64"/>
+      <c r="E6" s="69"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -3500,12 +3594,12 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="70" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3543,11 +3637,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3562,11 +3656,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3578,9 +3672,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -3615,12 +3709,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="70" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3657,11 +3751,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3676,11 +3770,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3692,9 +3786,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -3729,12 +3823,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="70" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3753,12 +3847,12 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="9" tint="-0.499984740745262"/>
+    <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3773,105 +3867,90 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="10" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="50" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+      <c r="B2" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="1:10" ht="240" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="B4" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="63" t="s">
-        <v>92</v>
+      <c r="B5" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="51" t="s">
+        <v>177</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="64"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="B6" s="70" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="E5:E6"/>
     <mergeCell ref="G2:I3"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
@@ -3884,11 +3963,13 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="9" tint="-0.499984740745262"/>
+    <tabColor rgb="FF0070C0"/>
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3902,90 +3983,90 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="10" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="50" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="49" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="B4" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="15" t="s">
-        <v>76</v>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="51" t="s">
+        <v>244</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="B6" s="70" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G2:I3"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="G2:I3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
@@ -4016,11 +4097,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -4035,25 +4116,25 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -4069,7 +4150,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -4077,7 +4158,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="60" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="3"/>
@@ -4085,7 +4166,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="5" t="s">
         <v>71</v>
       </c>
@@ -4093,13 +4174,13 @@
         <v>70</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="55"/>
+      <c r="E6" s="60"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>45</v>
@@ -4107,13 +4188,13 @@
       <c r="D7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="55"/>
+      <c r="E7" s="60"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="5"/>
       <c r="C8" s="7" t="s">
         <v>44</v>
@@ -4121,7 +4202,7 @@
       <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="55"/>
+      <c r="E8" s="60"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -4130,12 +4211,12 @@
       <c r="A9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4158,10 +4239,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4176,11 +4257,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4189,17 +4270,17 @@
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4211,54 +4292,69 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>227</v>
+      <c r="B4" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>75</v>
+      <c r="B5" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="15" t="s">
-        <v>76</v>
+      <c r="E5" s="68" t="s">
+        <v>92</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="69"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="B7" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="E5:E6"/>
     <mergeCell ref="G2:I3"/>
   </mergeCells>
   <hyperlinks>
@@ -4290,11 +4386,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4304,16 +4400,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4325,21 +4421,21 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>93</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>226</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4362,12 +4458,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="B6" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4390,7 +4486,9 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4404,11 +4502,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4418,16 +4516,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4439,21 +4537,21 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>97</v>
+        <v>227</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4476,12 +4574,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="B6" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4498,6 +4596,234 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="G2" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="G2:I3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="G2" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="G2:I3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -4518,11 +4844,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4537,11 +4863,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4553,9 +4879,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4579,7 +4905,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="60" t="s">
         <v>99</v>
       </c>
       <c r="H5" s="3"/>
@@ -4595,7 +4921,7 @@
         <v>73</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="55"/>
+      <c r="E6" s="60"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -4604,12 +4930,12 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4626,7 +4952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -4647,11 +4973,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4666,11 +4992,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4682,9 +5008,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4719,12 +5045,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4740,7 +5066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -4763,11 +5089,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4782,11 +5108,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4798,9 +5124,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4833,12 +5159,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4854,7 +5180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -4875,11 +5201,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4894,11 +5220,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4910,9 +5236,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4947,12 +5273,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4968,7 +5294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -4989,11 +5315,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5008,11 +5334,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5024,9 +5350,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5050,7 +5376,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="68" t="s">
         <v>162</v>
       </c>
       <c r="H5" s="3"/>
@@ -5066,7 +5392,7 @@
         <v>161</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="64"/>
+      <c r="E6" s="69"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5075,12 +5401,12 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5088,248 +5414,6 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="G2:I3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="83.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="G2" s="57" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="63" t="s">
-        <v>193</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
-      <c r="B6" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="64"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>192</v>
-      </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="G2:I3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B7:E7"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="83.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="G2" s="57" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="65" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="G2:I3"/>
-    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
@@ -5362,11 +5446,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="30" t="s">
         <v>47</v>
       </c>
@@ -5381,11 +5465,11 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -5397,9 +5481,9 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
@@ -5434,12 +5518,12 @@
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5456,6 +5540,248 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="G2" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="72"/>
+      <c r="B6" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="69"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="70" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B7:E7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="G2" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="70" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="B6:E6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -5478,68 +5804,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="43" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="42" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="G2" s="57" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="41" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="16" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="44" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="43" t="s">
         <v>196</v>
       </c>
       <c r="H5" s="3"/>
@@ -5547,15 +5873,15 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="70" t="s">
         <v>231</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5571,7 +5897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -5594,11 +5920,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5613,11 +5939,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5629,9 +5955,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5643,7 +5969,7 @@
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="71" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -5651,7 +5977,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="68" t="s">
         <v>111</v>
       </c>
       <c r="H5" s="3"/>
@@ -5659,7 +5985,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="5" t="s">
         <v>109</v>
       </c>
@@ -5667,7 +5993,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="64"/>
+      <c r="E6" s="69"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5676,12 +6002,12 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5720,11 +6046,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -5739,11 +6065,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -5755,9 +6081,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -5792,12 +6118,12 @@
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5821,7 +6147,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5836,11 +6162,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -5855,11 +6181,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -5871,9 +6197,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -5897,7 +6223,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="60" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="3"/>
@@ -5913,7 +6239,7 @@
         <v>70</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="55"/>
+      <c r="E6" s="60"/>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -5924,7 +6250,7 @@
       <c r="D7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="55"/>
+      <c r="E7" s="60"/>
     </row>
     <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -5935,18 +6261,18 @@
       <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="55"/>
+      <c r="E8" s="60"/>
     </row>
     <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5984,11 +6310,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6003,11 +6329,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6019,9 +6345,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6045,7 +6371,7 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="68" t="s">
         <v>148</v>
       </c>
       <c r="H5" s="3"/>
@@ -6061,7 +6387,7 @@
         <v>147</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="64"/>
+      <c r="E6" s="69"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -6070,12 +6396,12 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6113,11 +6439,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6132,11 +6458,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6148,9 +6474,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6181,12 +6507,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="70" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6223,11 +6549,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6242,11 +6568,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6258,9 +6584,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6295,12 +6621,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="70" t="s">
         <v>176</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6339,11 +6665,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6358,11 +6684,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6374,9 +6700,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6411,12 +6737,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="55" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
implement order create api
</commit_message>
<xml_diff>
--- a/design/API.xlsx
+++ b/design/API.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920" firstSheet="7" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -22,29 +22,30 @@
     <sheet name="client_07" sheetId="31" r:id="rId8"/>
     <sheet name="client_08" sheetId="33" r:id="rId9"/>
     <sheet name="client_09" sheetId="37" r:id="rId10"/>
-    <sheet name="deliveryman_01" sheetId="11" r:id="rId11"/>
-    <sheet name="deliveryman_02" sheetId="12" r:id="rId12"/>
-    <sheet name="deliveryman_03" sheetId="13" r:id="rId13"/>
-    <sheet name="deliveryman_04" sheetId="14" r:id="rId14"/>
-    <sheet name="deliveryman_05" sheetId="28" r:id="rId15"/>
-    <sheet name="deliveryman_06" sheetId="29" r:id="rId16"/>
-    <sheet name="deliveryman_07" sheetId="32" r:id="rId17"/>
-    <sheet name="deliveryman_08" sheetId="40" r:id="rId18"/>
-    <sheet name="deliveryman_09" sheetId="41" r:id="rId19"/>
-    <sheet name="order_01" sheetId="15" r:id="rId20"/>
-    <sheet name="order_02" sheetId="16" r:id="rId21"/>
-    <sheet name="order_03" sheetId="17" r:id="rId22"/>
-    <sheet name="order_04" sheetId="19" r:id="rId23"/>
-    <sheet name="order_05" sheetId="20" r:id="rId24"/>
-    <sheet name="order_06" sheetId="21" r:id="rId25"/>
-    <sheet name="order_07" sheetId="22" r:id="rId26"/>
-    <sheet name="order_08" sheetId="23" r:id="rId27"/>
-    <sheet name="order_09" sheetId="24" r:id="rId28"/>
-    <sheet name="order_10" sheetId="25" r:id="rId29"/>
-    <sheet name="notification_01" sheetId="35" r:id="rId30"/>
-    <sheet name="notification_02" sheetId="36" r:id="rId31"/>
-    <sheet name="notification_03" sheetId="39" r:id="rId32"/>
-    <sheet name="syslog_1" sheetId="26" r:id="rId33"/>
+    <sheet name="client_10" sheetId="42" r:id="rId11"/>
+    <sheet name="deliveryman_01" sheetId="11" r:id="rId12"/>
+    <sheet name="deliveryman_02" sheetId="12" r:id="rId13"/>
+    <sheet name="deliveryman_03" sheetId="13" r:id="rId14"/>
+    <sheet name="deliveryman_04" sheetId="14" r:id="rId15"/>
+    <sheet name="deliveryman_05" sheetId="28" r:id="rId16"/>
+    <sheet name="deliveryman_06" sheetId="29" r:id="rId17"/>
+    <sheet name="deliveryman_07" sheetId="32" r:id="rId18"/>
+    <sheet name="deliveryman_08" sheetId="40" r:id="rId19"/>
+    <sheet name="deliveryman_09" sheetId="41" r:id="rId20"/>
+    <sheet name="order_01" sheetId="15" r:id="rId21"/>
+    <sheet name="order_02" sheetId="16" r:id="rId22"/>
+    <sheet name="order_03" sheetId="17" r:id="rId23"/>
+    <sheet name="order_04" sheetId="19" r:id="rId24"/>
+    <sheet name="order_05" sheetId="20" r:id="rId25"/>
+    <sheet name="order_06" sheetId="21" r:id="rId26"/>
+    <sheet name="order_07" sheetId="22" r:id="rId27"/>
+    <sheet name="order_08" sheetId="23" r:id="rId28"/>
+    <sheet name="order_09" sheetId="24" r:id="rId29"/>
+    <sheet name="order_10" sheetId="25" r:id="rId30"/>
+    <sheet name="notification_01" sheetId="35" r:id="rId31"/>
+    <sheet name="notification_02" sheetId="36" r:id="rId32"/>
+    <sheet name="notification_03" sheetId="39" r:id="rId33"/>
+    <sheet name="syslog_1" sheetId="26" r:id="rId34"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="248">
   <si>
     <t xml:space="preserve">get order list by order status </t>
   </si>
@@ -1572,9 +1573,6 @@
     <t>deliveryman/updateLocation</t>
   </si>
   <si>
-    <t>update location of delivery man by ID.</t>
-  </si>
-  <si>
     <t>{
     deliverymanID: int,
     locationLatitude string,
@@ -1595,6 +1593,21 @@
     "message": "update Success.",
     "data": [ ]
 }</t>
+  </si>
+  <si>
+    <t>update location info of delivery man by ID.</t>
+  </si>
+  <si>
+    <t>client/updateFcmToken</t>
+  </si>
+  <si>
+    <t>{
+    clientID: int,
+    fcmToken: string
+}</t>
+  </si>
+  <si>
+    <t>client_10</t>
   </si>
 </sst>
 </file>
@@ -1687,7 +1700,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1835,6 +1848,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1930,9 +1952,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1964,11 +1983,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2041,6 +2056,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2326,10 +2350,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,13 +2375,13 @@
       <c r="C1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="57"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="70" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2366,7 +2390,7 @@
       <c r="C2" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="37"/>
       <c r="G2" s="19" t="s">
         <v>113</v>
       </c>
@@ -2375,14 +2399,14 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
-      <c r="B3" s="35" t="s">
+      <c r="A3" s="71"/>
+      <c r="B3" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="37"/>
       <c r="G3" s="4" t="s">
         <v>115</v>
       </c>
@@ -2391,14 +2415,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
+      <c r="A4" s="71"/>
       <c r="B4" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="37"/>
       <c r="G4" s="4" t="s">
         <v>117</v>
       </c>
@@ -2407,14 +2431,14 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
+      <c r="A5" s="71"/>
       <c r="B5" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="37"/>
       <c r="G5" s="4" t="s">
         <v>119</v>
       </c>
@@ -2423,431 +2447,444 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="20" t="s">
         <v>141</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="38"/>
+      <c r="D6" s="37"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="20" t="s">
         <v>168</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="37"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="20" t="s">
         <v>170</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="D8" s="38"/>
+      <c r="D8" s="37"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="71"/>
       <c r="B9" s="20" t="s">
         <v>183</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="D9" s="38"/>
+      <c r="D9" s="37"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
+      <c r="A10" s="71"/>
+      <c r="B10" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="72"/>
+      <c r="B11" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D11" s="36"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C12" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="G11" s="4" t="s">
+      <c r="D12" s="37"/>
+      <c r="G12" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
-      <c r="B12" s="7" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="51"/>
+      <c r="B13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="G12" s="4" t="s">
+      <c r="D13" s="37"/>
+      <c r="G13" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="7" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="51"/>
+      <c r="B14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="D14" s="38"/>
+      <c r="D14" s="37"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
-      <c r="B15" s="20" t="s">
-        <v>151</v>
+      <c r="A15" s="51"/>
+      <c r="B15" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D15" s="38"/>
+        <v>221</v>
+      </c>
+      <c r="D15" s="37"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="20" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D16" s="38"/>
+        <v>152</v>
+      </c>
+      <c r="D16" s="37"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="20" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D17" s="38"/>
+        <v>164</v>
+      </c>
+      <c r="D17" s="37"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="47" t="s">
-        <v>234</v>
+      <c r="A18" s="51"/>
+      <c r="B18" s="20" t="s">
+        <v>172</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="D18" s="38"/>
+        <v>173</v>
+      </c>
+      <c r="D18" s="37"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="47" t="s">
-        <v>239</v>
+      <c r="A19" s="51"/>
+      <c r="B19" s="45" t="s">
+        <v>234</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="D19" s="38"/>
+        <v>235</v>
+      </c>
+      <c r="D19" s="37"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="55"/>
+      <c r="B20" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="G20" s="19" t="s">
+      <c r="D21" s="37"/>
+      <c r="G21" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H21" s="19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="55"/>
-      <c r="B21" s="7" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="52"/>
+      <c r="B22" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C22" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="G21" s="4" t="s">
+      <c r="D22" s="37"/>
+      <c r="G22" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="7" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="52"/>
+      <c r="B23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="38"/>
-      <c r="G22" s="4" t="s">
+      <c r="D23" s="37"/>
+      <c r="G23" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
-      <c r="B23" s="7" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="52"/>
+      <c r="B24" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C24" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="38"/>
-      <c r="G23" s="4" t="s">
+      <c r="D24" s="37"/>
+      <c r="G24" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="55"/>
-      <c r="B24" s="7" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="52"/>
+      <c r="B25" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C25" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="38"/>
-      <c r="G24" s="4" t="s">
+      <c r="D25" s="37"/>
+      <c r="G25" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
-      <c r="B25" s="7" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="52"/>
+      <c r="B26" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C26" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="G25" s="4" t="s">
+      <c r="D26" s="37"/>
+      <c r="G26" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
-      <c r="B26" s="7" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="52"/>
+      <c r="B27" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C27" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="38"/>
-      <c r="G26" s="4" t="s">
+      <c r="D27" s="37"/>
+      <c r="G27" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
-      <c r="B27" s="7" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="52"/>
+      <c r="B28" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C28" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="G27" s="4" t="s">
+      <c r="D28" s="37"/>
+      <c r="G28" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
-      <c r="B28" s="7" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="52"/>
+      <c r="B29" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C29" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="38"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
-      <c r="B29" s="7" t="s">
+      <c r="D29" s="37"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="52"/>
+      <c r="B30" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C30" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="38"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
+      <c r="D30" s="37"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B31" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C31" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="D30" s="38"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
-      <c r="B31" s="20" t="s">
+      <c r="D31" s="37"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="51"/>
+      <c r="B32" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C32" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="D31" s="38"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="40" t="s">
+      <c r="D32" s="37"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="51"/>
+      <c r="B33" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C33" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="D32" s="38"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="D33" s="37"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C34" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="38"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="39"/>
-      <c r="C35" t="s">
+      <c r="D34" s="37"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="38"/>
+      <c r="C36" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="36"/>
-      <c r="C36" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="35"/>
+      <c r="C37" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="38"/>
-      <c r="C37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="37"/>
+      <c r="C38" t="s">
         <v>210</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A20:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A21:A30"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A2:A11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" location="client_01!A1" display="client/get"/>
     <hyperlink ref="C4" location="client_03!A1" display="client/savelocations"/>
     <hyperlink ref="C5" location="client_04!A1" display="client/list"/>
-    <hyperlink ref="C11" location="deliveryman_01!A1" display="deliveryman/get"/>
-    <hyperlink ref="C12" location="deliveryman_02!A1" display="deliveryman/totalcount"/>
-    <hyperlink ref="C13" location="deliveryman_03!A1" display="deliveryman/list"/>
-    <hyperlink ref="C14" location="deliveryman_04!A1" display="deliveryman/save"/>
-    <hyperlink ref="C20" location="order_01!A1" display="order/create"/>
-    <hyperlink ref="C21" location="order_02!A1" display="order/send"/>
-    <hyperlink ref="C22" location="order_03!A1" display="order/cancel"/>
-    <hyperlink ref="C23" location="order_04!A1" display="order/receive"/>
-    <hyperlink ref="C24" location="order_05!A1" display="order/rate"/>
-    <hyperlink ref="C25" location="order_06!A1" display="order/acceptrequest"/>
-    <hyperlink ref="C26" location="order_07!A1" display="orders/totalcount"/>
-    <hyperlink ref="C27" location="order_08!A1" display="order/totalearning"/>
-    <hyperlink ref="C28" location="order_09!A1" display="order/dailycount"/>
-    <hyperlink ref="C29" location="order_10!A1" display="order/list"/>
-    <hyperlink ref="C33" location="syslog_1!A1" display="syslog/list"/>
+    <hyperlink ref="C12" location="deliveryman_01!A1" display="deliveryman/get"/>
+    <hyperlink ref="C13" location="deliveryman_02!A1" display="deliveryman/totalcount"/>
+    <hyperlink ref="C14" location="deliveryman_03!A1" display="deliveryman/list"/>
+    <hyperlink ref="C15" location="deliveryman_04!A1" display="deliveryman/save"/>
+    <hyperlink ref="C21" location="order_01!A1" display="order/create"/>
+    <hyperlink ref="C22" location="order_02!A1" display="order/send"/>
+    <hyperlink ref="C23" location="order_03!A1" display="order/cancel"/>
+    <hyperlink ref="C24" location="order_04!A1" display="order/receive"/>
+    <hyperlink ref="C25" location="order_05!A1" display="order/rate"/>
+    <hyperlink ref="C26" location="order_06!A1" display="order/acceptrequest"/>
+    <hyperlink ref="C27" location="order_07!A1" display="orders/totalcount"/>
+    <hyperlink ref="C28" location="order_08!A1" display="order/totalearning"/>
+    <hyperlink ref="C29" location="order_09!A1" display="order/dailycount"/>
+    <hyperlink ref="C30" location="order_10!A1" display="order/list"/>
+    <hyperlink ref="C34" location="syslog_1!A1" display="syslog/list"/>
     <hyperlink ref="C6" location="client_05!A1" display="client/orderlist"/>
-    <hyperlink ref="C15" location="deliveryman_05!A1" display="deliveryman/orderlist"/>
-    <hyperlink ref="C16" location="deliveryman_06!A1" display="deliveryman/changeState"/>
+    <hyperlink ref="C16" location="deliveryman_05!A1" display="deliveryman/orderlist"/>
+    <hyperlink ref="C17" location="deliveryman_06!A1" display="deliveryman/changeState"/>
     <hyperlink ref="C7" location="client_06!A1" display="client/totalcount"/>
-    <hyperlink ref="C17" location="deliveryman_07!A1" display="deliveryman/delete"/>
+    <hyperlink ref="C18" location="deliveryman_07!A1" display="deliveryman/delete"/>
     <hyperlink ref="C8" location="client_07!A1" display="client/delete"/>
     <hyperlink ref="C9" location="client_08!A1" display="client/update"/>
-    <hyperlink ref="C31" location="notification_02!A1" display="notification/delete"/>
-    <hyperlink ref="C30" location="notification_01!A1" display="notification/list"/>
+    <hyperlink ref="C32" location="notification_02!A1" display="notification/delete"/>
+    <hyperlink ref="C31" location="notification_01!A1" display="notification/list"/>
     <hyperlink ref="C10" location="client_09!A1" display="client/phonecheck"/>
-    <hyperlink ref="C32" location="notification_03!A1" display="notification/create"/>
-    <hyperlink ref="C18" location="deliveryman_08!A1" display="deliveryman/updateFcmToken"/>
+    <hyperlink ref="C33" location="notification_03!A1" display="notification/create"/>
+    <hyperlink ref="C19" location="deliveryman_08!A1" display="deliveryman/updateFcmToken"/>
+    <hyperlink ref="C20" location="deliveryman_09!A1" display="deliveryman/updateLocation"/>
+    <hyperlink ref="C11" location="client_10!A1" display="client/updateFcmToken"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2857,7 +2894,7 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
+    <tabColor theme="5" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -2875,11 +2912,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="30" t="s">
         <v>47</v>
       </c>
@@ -2894,11 +2931,11 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -2910,9 +2947,9 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
@@ -2947,12 +2984,12 @@
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="52" t="s">
         <v>202</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2968,6 +3005,122 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="G2" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
+    </row>
+    <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="B6:E6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -2990,11 +3143,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3009,11 +3162,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3025,9 +3178,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3043,7 +3196,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="56" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3051,7 +3204,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="57" t="s">
         <v>82</v>
       </c>
       <c r="H5" s="3"/>
@@ -3059,7 +3212,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="5" t="s">
         <v>80</v>
       </c>
@@ -3067,13 +3220,13 @@
         <v>81</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="60"/>
+      <c r="E6" s="57"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -3081,7 +3234,7 @@
       <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="60"/>
+      <c r="E7" s="57"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -3090,12 +3243,12 @@
       <c r="A8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3113,7 +3266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -3134,11 +3287,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3153,11 +3306,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3169,9 +3322,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3206,12 +3359,12 @@
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3227,7 +3380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -3248,11 +3401,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3267,11 +3420,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3283,9 +3436,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3301,7 +3454,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="56" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3309,7 +3462,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="57" t="s">
         <v>82</v>
       </c>
       <c r="H5" s="3"/>
@@ -3317,7 +3470,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="5" t="s">
         <v>80</v>
       </c>
@@ -3325,13 +3478,13 @@
         <v>89</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="60"/>
+      <c r="E6" s="57"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -3339,7 +3492,7 @@
       <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="60"/>
+      <c r="E7" s="57"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -3348,12 +3501,12 @@
       <c r="A8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3371,7 +3524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -3394,11 +3547,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3413,11 +3566,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3429,9 +3582,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3466,12 +3619,12 @@
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3487,7 +3640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -3508,11 +3661,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3527,11 +3680,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3543,9 +3696,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -3569,7 +3722,7 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="65" t="s">
         <v>148</v>
       </c>
       <c r="H5" s="3"/>
@@ -3585,7 +3738,7 @@
         <v>147</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="69"/>
+      <c r="E6" s="66"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -3594,12 +3747,12 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3607,120 +3760,6 @@
     <mergeCell ref="G2:I3"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="B7:E7"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF0070C0"/>
-  </sheetPr>
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="83.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="G2" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="70" t="s">
-        <v>166</v>
-      </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="G2:I3"/>
-    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
@@ -3751,11 +3790,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3765,16 +3804,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3786,9 +3825,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -3813,7 +3852,7 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="25" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -3823,12 +3862,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="B6" s="67" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3851,9 +3890,7 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3867,68 +3904,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="50" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="21" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="G2" s="62" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-    </row>
-    <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="B3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
+        <v>153</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="16" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="51" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="25" t="s">
         <v>177</v>
       </c>
       <c r="H5" s="3"/>
@@ -3936,15 +3973,15 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
-        <v>238</v>
-      </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="B6" s="67" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3967,8 +4004,8 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3983,84 +4020,84 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="50" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="47" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="46" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="G2" s="62" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="46" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
+        <v>236</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="16" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="51" t="s">
-        <v>244</v>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="48" t="s">
+        <v>177</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
-        <v>241</v>
-      </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="B6" s="67" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4097,11 +4134,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -4116,25 +4153,25 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -4150,7 +4187,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="56" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -4158,7 +4195,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="57" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="3"/>
@@ -4166,7 +4203,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="5" t="s">
         <v>71</v>
       </c>
@@ -4174,13 +4211,13 @@
         <v>70</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="60"/>
+      <c r="E6" s="57"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>45</v>
@@ -4188,13 +4225,13 @@
       <c r="D7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="60"/>
+      <c r="E7" s="57"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="5"/>
       <c r="C8" s="7" t="s">
         <v>44</v>
@@ -4202,7 +4239,7 @@
       <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="60"/>
+      <c r="E8" s="57"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -4211,12 +4248,12 @@
       <c r="A9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4235,6 +4272,122 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="G2" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
+    </row>
+    <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="16" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="B6:E6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -4257,11 +4410,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4276,11 +4429,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4292,9 +4445,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4313,12 +4466,12 @@
       <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>90</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="65" t="s">
         <v>92</v>
       </c>
       <c r="H5" s="3"/>
@@ -4334,7 +4487,7 @@
         <v>73</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="69"/>
+      <c r="E6" s="66"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -4343,12 +4496,12 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4365,7 +4518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -4386,11 +4539,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4405,11 +4558,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4421,9 +4574,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4458,12 +4611,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4479,7 +4632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -4502,11 +4655,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4521,11 +4674,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4537,9 +4690,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4574,126 +4727,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="G2:I3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="9" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="83.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="16" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="70" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4716,7 +4755,7 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4730,11 +4769,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4744,16 +4783,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4765,21 +4804,21 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>97</v>
+      <c r="B4" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>96</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4802,12 +4841,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="B6" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4824,6 +4863,120 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="G2" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
+    </row>
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="G2:I3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -4844,11 +4997,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4863,11 +5016,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4879,9 +5032,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4905,7 +5058,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="57" t="s">
         <v>99</v>
       </c>
       <c r="H5" s="3"/>
@@ -4921,7 +5074,7 @@
         <v>73</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="60"/>
+      <c r="E6" s="57"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -4930,12 +5083,12 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4952,7 +5105,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -4973,11 +5126,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4992,11 +5145,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5008,9 +5161,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5045,12 +5198,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5066,7 +5219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -5089,11 +5242,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5108,11 +5261,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5124,9 +5277,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5159,12 +5312,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5180,7 +5333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -5201,11 +5354,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5220,11 +5373,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5236,9 +5389,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5273,146 +5426,17 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="G2:I3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="9" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="83.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-    </row>
-    <row r="4" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" ht="225" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="69"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B7:E7"/>
     <mergeCell ref="G2:I3"/>
   </mergeCells>
   <hyperlinks>
@@ -5446,11 +5470,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="30" t="s">
         <v>47</v>
       </c>
@@ -5465,11 +5489,11 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -5481,9 +5505,9 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
@@ -5518,12 +5542,12 @@
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5540,6 +5564,135 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="G2" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
+    </row>
+    <row r="4" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="66"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="G2:I3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -5560,11 +5713,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -5579,11 +5732,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -5595,9 +5748,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -5611,7 +5764,7 @@
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="68" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -5619,7 +5772,7 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="65" t="s">
         <v>193</v>
       </c>
       <c r="H5" s="3"/>
@@ -5627,7 +5780,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="24" t="s">
         <v>190</v>
       </c>
@@ -5635,7 +5788,7 @@
         <v>191</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="69"/>
+      <c r="E6" s="66"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5644,12 +5797,12 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5667,7 +5820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -5688,11 +5841,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -5707,11 +5860,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -5723,9 +5876,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -5760,12 +5913,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="67" t="s">
         <v>197</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5781,7 +5934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -5804,68 +5957,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="42" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="41" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="40" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="G2" s="62" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="40" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="16" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="43" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="42" t="s">
         <v>196</v>
       </c>
       <c r="H5" s="3"/>
@@ -5873,15 +6026,15 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="67" t="s">
         <v>231</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5897,7 +6050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -5920,11 +6073,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5939,11 +6092,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5955,9 +6108,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5969,7 +6122,7 @@
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="68" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -5977,7 +6130,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="65" t="s">
         <v>111</v>
       </c>
       <c r="H5" s="3"/>
@@ -5985,7 +6138,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="5" t="s">
         <v>109</v>
       </c>
@@ -5993,7 +6146,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="69"/>
+      <c r="E6" s="66"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -6002,12 +6155,12 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6046,11 +6199,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -6065,11 +6218,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -6081,9 +6234,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -6118,12 +6271,12 @@
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6162,11 +6315,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -6181,11 +6334,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -6197,9 +6350,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -6223,7 +6376,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="57" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="3"/>
@@ -6239,7 +6392,7 @@
         <v>70</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="60"/>
+      <c r="E6" s="57"/>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -6250,7 +6403,7 @@
       <c r="D7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="60"/>
+      <c r="E7" s="57"/>
     </row>
     <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -6261,18 +6414,18 @@
       <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="60"/>
+      <c r="E8" s="57"/>
     </row>
     <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6310,11 +6463,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6329,11 +6482,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6345,9 +6498,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6371,7 +6524,7 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="65" t="s">
         <v>148</v>
       </c>
       <c r="H5" s="3"/>
@@ -6387,7 +6540,7 @@
         <v>147</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="69"/>
+      <c r="E6" s="66"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -6396,12 +6549,12 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="67" t="s">
         <v>156</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6439,11 +6592,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6458,11 +6611,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6474,9 +6627,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6507,12 +6660,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="67" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6549,11 +6702,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6568,11 +6721,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6584,9 +6737,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6621,12 +6774,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="67" t="s">
         <v>176</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6665,11 +6818,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6684,11 +6837,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6700,9 +6853,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6737,12 +6890,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
implement in progress page logic
</commit_message>
<xml_diff>
--- a/design/API.xlsx
+++ b/design/API.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920" firstSheet="14" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -42,10 +42,11 @@
     <sheet name="order_08" sheetId="23" r:id="rId28"/>
     <sheet name="order_09" sheetId="24" r:id="rId29"/>
     <sheet name="order_10" sheetId="25" r:id="rId30"/>
-    <sheet name="notification_01" sheetId="35" r:id="rId31"/>
-    <sheet name="notification_02" sheetId="36" r:id="rId32"/>
-    <sheet name="notification_03" sheetId="39" r:id="rId33"/>
-    <sheet name="syslog_1" sheetId="26" r:id="rId34"/>
+    <sheet name="order_11" sheetId="43" r:id="rId31"/>
+    <sheet name="notification_01" sheetId="35" r:id="rId32"/>
+    <sheet name="notification_02" sheetId="36" r:id="rId33"/>
+    <sheet name="notification_03" sheetId="39" r:id="rId34"/>
+    <sheet name="syslog_1" sheetId="26" r:id="rId35"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="253">
   <si>
     <t xml:space="preserve">get order list by order status </t>
   </si>
@@ -1608,6 +1609,27 @@
   </si>
   <si>
     <t>client_10</t>
+  </si>
+  <si>
+    <t>order_11</t>
+  </si>
+  <si>
+    <t>order/inprogress</t>
+  </si>
+  <si>
+    <t>{
+    sender: string,
+    receiver: string,
+}</t>
+  </si>
+  <si>
+    <t>{
+    "sender": "sender ID",
+    "receiver": "receiver's phone",
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get inprogress order list by sender id and receiver phone </t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1885,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1981,6 +2003,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2350,10 +2375,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,13 +2400,13 @@
       <c r="C1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="54"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="71" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2399,7 +2424,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="71"/>
+      <c r="A3" s="72"/>
       <c r="B3" s="34" t="s">
         <v>50</v>
       </c>
@@ -2415,7 +2440,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="71"/>
+      <c r="A4" s="72"/>
       <c r="B4" s="7" t="s">
         <v>51</v>
       </c>
@@ -2431,7 +2456,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="71"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="7" t="s">
         <v>52</v>
       </c>
@@ -2447,7 +2472,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="20" t="s">
         <v>141</v>
       </c>
@@ -2459,7 +2484,7 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="20" t="s">
         <v>168</v>
       </c>
@@ -2471,7 +2496,7 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="20" t="s">
         <v>170</v>
       </c>
@@ -2483,7 +2508,7 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="20" t="s">
         <v>183</v>
       </c>
@@ -2495,7 +2520,7 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="4" t="s">
         <v>198</v>
       </c>
@@ -2505,7 +2530,7 @@
       <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="72"/>
+      <c r="A11" s="73"/>
       <c r="B11" s="4" t="s">
         <v>247</v>
       </c>
@@ -2515,7 +2540,7 @@
       <c r="D11" s="36"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="51" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2533,7 +2558,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="7" t="s">
         <v>54</v>
       </c>
@@ -2549,7 +2574,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="7" t="s">
         <v>55</v>
       </c>
@@ -2561,7 +2586,7 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="7" t="s">
         <v>56</v>
       </c>
@@ -2573,7 +2598,7 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="20" t="s">
         <v>151</v>
       </c>
@@ -2585,7 +2610,7 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
+      <c r="A17" s="52"/>
       <c r="B17" s="20" t="s">
         <v>163</v>
       </c>
@@ -2597,7 +2622,7 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
+      <c r="A18" s="52"/>
       <c r="B18" s="20" t="s">
         <v>172</v>
       </c>
@@ -2609,8 +2634,8 @@
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
-      <c r="B19" s="45" t="s">
+      <c r="A19" s="52"/>
+      <c r="B19" s="46" t="s">
         <v>234</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -2621,8 +2646,8 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="55"/>
-      <c r="B20" s="45" t="s">
+      <c r="A20" s="56"/>
+      <c r="B20" s="46" t="s">
         <v>239</v>
       </c>
       <c r="C20" s="17" t="s">
@@ -2633,7 +2658,7 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="53" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -2651,7 +2676,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="7" t="s">
         <v>58</v>
       </c>
@@ -2667,7 +2692,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="7" t="s">
         <v>59</v>
       </c>
@@ -2683,7 +2708,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="7" t="s">
         <v>60</v>
       </c>
@@ -2699,7 +2724,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="7" t="s">
         <v>61</v>
       </c>
@@ -2715,7 +2740,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="7" t="s">
         <v>62</v>
       </c>
@@ -2731,7 +2756,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="7" t="s">
         <v>63</v>
       </c>
@@ -2747,7 +2772,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
+      <c r="A28" s="53"/>
       <c r="B28" s="7" t="s">
         <v>64</v>
       </c>
@@ -2763,7 +2788,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
+      <c r="A29" s="53"/>
       <c r="B29" s="7" t="s">
         <v>65</v>
       </c>
@@ -2773,7 +2798,7 @@
       <c r="D29" s="37"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
+      <c r="A30" s="53"/>
       <c r="B30" s="7" t="s">
         <v>66</v>
       </c>
@@ -2783,70 +2808,80 @@
       <c r="D30" s="37"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="50" t="s">
+      <c r="A31" s="45"/>
+      <c r="B31" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="D31" s="37"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B32" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C32" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="D31" s="37"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="51"/>
-      <c r="B32" s="20" t="s">
+      <c r="D32" s="37"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="52"/>
+      <c r="B33" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C33" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="D32" s="37"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="51"/>
-      <c r="B33" s="39" t="s">
+      <c r="D33" s="37"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="52"/>
+      <c r="B34" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C34" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="D33" s="37"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="D34" s="37"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C35" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="37"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="38"/>
-      <c r="C36" t="s">
+      <c r="D35" s="37"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="38"/>
+      <c r="C37" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="35"/>
-      <c r="C37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="35"/>
+      <c r="C38" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="37"/>
-      <c r="C38" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="37"/>
+      <c r="C39" t="s">
         <v>210</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A32:A34"/>
     <mergeCell ref="A21:A30"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A12:A20"/>
@@ -2870,7 +2905,7 @@
     <hyperlink ref="C28" location="order_08!A1" display="order/totalearning"/>
     <hyperlink ref="C29" location="order_09!A1" display="order/dailycount"/>
     <hyperlink ref="C30" location="order_10!A1" display="order/list"/>
-    <hyperlink ref="C34" location="syslog_1!A1" display="syslog/list"/>
+    <hyperlink ref="C35" location="syslog_1!A1" display="syslog/list"/>
     <hyperlink ref="C6" location="client_05!A1" display="client/orderlist"/>
     <hyperlink ref="C16" location="deliveryman_05!A1" display="deliveryman/orderlist"/>
     <hyperlink ref="C17" location="deliveryman_06!A1" display="deliveryman/changeState"/>
@@ -2878,13 +2913,14 @@
     <hyperlink ref="C18" location="deliveryman_07!A1" display="deliveryman/delete"/>
     <hyperlink ref="C8" location="client_07!A1" display="client/delete"/>
     <hyperlink ref="C9" location="client_08!A1" display="client/update"/>
-    <hyperlink ref="C32" location="notification_02!A1" display="notification/delete"/>
-    <hyperlink ref="C31" location="notification_01!A1" display="notification/list"/>
+    <hyperlink ref="C33" location="notification_02!A1" display="notification/delete"/>
+    <hyperlink ref="C32" location="notification_01!A1" display="notification/list"/>
     <hyperlink ref="C10" location="client_09!A1" display="client/phonecheck"/>
-    <hyperlink ref="C33" location="notification_03!A1" display="notification/create"/>
+    <hyperlink ref="C34" location="notification_03!A1" display="notification/create"/>
     <hyperlink ref="C19" location="deliveryman_08!A1" display="deliveryman/updateFcmToken"/>
     <hyperlink ref="C20" location="deliveryman_09!A1" display="deliveryman/updateLocation"/>
     <hyperlink ref="C11" location="client_10!A1" display="client/updateFcmToken"/>
+    <hyperlink ref="C31" location="order_11!A1" display="order/inprogress"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2912,11 +2948,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="30" t="s">
         <v>47</v>
       </c>
@@ -2931,11 +2967,11 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -2947,9 +2983,9 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
@@ -2984,12 +3020,12 @@
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="53" t="s">
         <v>202</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3027,68 +3063,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="47" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="48" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="G2" s="59" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="48" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="49" t="s">
         <v>177</v>
       </c>
       <c r="H5" s="3"/>
@@ -3096,15 +3132,15 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3143,11 +3179,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3162,11 +3198,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3178,9 +3214,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3196,7 +3232,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="57" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3204,7 +3240,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="58" t="s">
         <v>82</v>
       </c>
       <c r="H5" s="3"/>
@@ -3212,7 +3248,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="5" t="s">
         <v>80</v>
       </c>
@@ -3220,13 +3256,13 @@
         <v>81</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="57"/>
+      <c r="E6" s="58"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -3234,7 +3270,7 @@
       <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="57"/>
+      <c r="E7" s="58"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -3243,12 +3279,12 @@
       <c r="A8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3287,11 +3323,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3306,11 +3342,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3322,9 +3358,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3359,12 +3395,12 @@
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3401,11 +3437,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3420,11 +3456,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3436,9 +3472,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3454,7 +3490,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="57" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3462,7 +3498,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="58" t="s">
         <v>82</v>
       </c>
       <c r="H5" s="3"/>
@@ -3470,7 +3506,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="5" t="s">
         <v>80</v>
       </c>
@@ -3478,13 +3514,13 @@
         <v>89</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="57"/>
+      <c r="E6" s="58"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -3492,7 +3528,7 @@
       <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="57"/>
+      <c r="E7" s="58"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -3501,12 +3537,12 @@
       <c r="A8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3547,11 +3583,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3566,11 +3602,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3582,9 +3618,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3619,12 +3655,12 @@
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3661,11 +3697,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3680,11 +3716,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3696,9 +3732,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -3722,7 +3758,7 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="66" t="s">
         <v>148</v>
       </c>
       <c r="H5" s="3"/>
@@ -3738,7 +3774,7 @@
         <v>147</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="66"/>
+      <c r="E6" s="67"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -3747,12 +3783,12 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3790,11 +3826,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3809,11 +3845,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3825,9 +3861,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -3862,12 +3898,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3904,11 +3940,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3923,11 +3959,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3939,9 +3975,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -3976,12 +4012,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4020,68 +4056,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="47" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="48" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="G2" s="59" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="48" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="49" t="s">
         <v>177</v>
       </c>
       <c r="H5" s="3"/>
@@ -4089,15 +4125,15 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4134,11 +4170,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -4153,11 +4189,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -4169,9 +4205,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -4187,7 +4223,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="57" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -4195,7 +4231,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="58" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="3"/>
@@ -4203,7 +4239,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="5" t="s">
         <v>71</v>
       </c>
@@ -4211,13 +4247,13 @@
         <v>70</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="57"/>
+      <c r="E6" s="58"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>45</v>
@@ -4225,13 +4261,13 @@
       <c r="D7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="57"/>
+      <c r="E7" s="58"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="5"/>
       <c r="C8" s="7" t="s">
         <v>44</v>
@@ -4239,7 +4275,7 @@
       <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="57"/>
+      <c r="E8" s="58"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -4248,12 +4284,12 @@
       <c r="A9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4294,68 +4330,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="47" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="48" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="G2" s="59" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="48" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="49" t="s">
         <v>243</v>
       </c>
       <c r="H5" s="3"/>
@@ -4363,15 +4399,15 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>244</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4410,11 +4446,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4429,11 +4465,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4445,9 +4481,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4471,7 +4507,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="66" t="s">
         <v>92</v>
       </c>
       <c r="H5" s="3"/>
@@ -4487,7 +4523,7 @@
         <v>73</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="66"/>
+      <c r="E6" s="67"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -4496,12 +4532,12 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4539,11 +4575,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4558,11 +4594,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4574,9 +4610,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4611,12 +4647,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4655,11 +4691,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4674,11 +4710,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4690,9 +4726,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4727,12 +4763,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4769,11 +4805,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4788,11 +4824,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4804,9 +4840,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4841,12 +4877,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4883,11 +4919,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4902,11 +4938,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4918,9 +4954,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4955,12 +4991,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4997,11 +5033,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5016,11 +5052,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5032,9 +5068,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5058,7 +5094,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="58" t="s">
         <v>99</v>
       </c>
       <c r="H5" s="3"/>
@@ -5074,7 +5110,7 @@
         <v>73</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="57"/>
+      <c r="E6" s="58"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5083,12 +5119,12 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5126,11 +5162,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5145,11 +5181,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5161,9 +5197,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5198,12 +5234,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5242,11 +5278,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5261,11 +5297,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5277,9 +5313,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5312,12 +5348,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5354,11 +5390,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5373,11 +5409,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5389,9 +5425,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5426,12 +5462,12 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5470,11 +5506,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="30" t="s">
         <v>47</v>
       </c>
@@ -5489,11 +5525,11 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -5505,9 +5541,9 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
@@ -5542,12 +5578,12 @@
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5584,11 +5620,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5603,11 +5639,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5619,9 +5655,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -5645,7 +5681,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="66" t="s">
         <v>162</v>
       </c>
       <c r="H5" s="3"/>
@@ -5661,7 +5697,7 @@
         <v>161</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="66"/>
+      <c r="E6" s="67"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5670,12 +5706,12 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5693,6 +5729,137 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="G2" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
+    </row>
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="67"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="68" t="s">
+        <v>252</v>
+      </c>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B7:E7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2:I3" location="Contents!A1" display="Back to Content"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -5713,11 +5880,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -5732,11 +5899,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -5748,9 +5915,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -5764,7 +5931,7 @@
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="69" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -5772,7 +5939,7 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="66" t="s">
         <v>193</v>
       </c>
       <c r="H5" s="3"/>
@@ -5780,7 +5947,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="24" t="s">
         <v>190</v>
       </c>
@@ -5788,7 +5955,7 @@
         <v>191</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="66"/>
+      <c r="E6" s="67"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5797,12 +5964,12 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>192</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5820,7 +5987,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -5841,11 +6008,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -5860,11 +6027,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -5876,9 +6043,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -5913,12 +6080,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>197</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5934,7 +6101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -5957,11 +6124,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="41" t="s">
         <v>47</v>
       </c>
@@ -5976,11 +6143,11 @@
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -5992,9 +6159,9 @@
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
@@ -6029,12 +6196,12 @@
       <c r="A6" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>231</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6050,7 +6217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -6073,11 +6240,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -6092,11 +6259,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -6108,9 +6275,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -6122,7 +6289,7 @@
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="69" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -6130,7 +6297,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="66" t="s">
         <v>111</v>
       </c>
       <c r="H5" s="3"/>
@@ -6138,7 +6305,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="5" t="s">
         <v>109</v>
       </c>
@@ -6146,7 +6313,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="66"/>
+      <c r="E6" s="67"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -6155,12 +6322,12 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6199,11 +6366,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -6218,11 +6385,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -6234,9 +6401,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -6271,12 +6438,12 @@
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6315,11 +6482,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -6334,11 +6501,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -6350,9 +6517,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -6376,7 +6543,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="58" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="3"/>
@@ -6392,7 +6559,7 @@
         <v>70</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="57"/>
+      <c r="E6" s="58"/>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -6403,7 +6570,7 @@
       <c r="D7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="57"/>
+      <c r="E7" s="58"/>
     </row>
     <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -6414,18 +6581,18 @@
       <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="57"/>
+      <c r="E8" s="58"/>
     </row>
     <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6463,11 +6630,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6482,11 +6649,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6498,9 +6665,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6524,7 +6691,7 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="66" t="s">
         <v>148</v>
       </c>
       <c r="H5" s="3"/>
@@ -6540,7 +6707,7 @@
         <v>147</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="66"/>
+      <c r="E6" s="67"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -6549,12 +6716,12 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6592,11 +6759,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6611,11 +6778,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6627,9 +6794,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6660,12 +6827,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6702,11 +6869,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6721,11 +6888,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6737,9 +6904,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6774,12 +6941,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>176</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6818,11 +6985,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6837,11 +7004,11 @@
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6853,9 +7020,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6890,12 +7057,12 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
changed order update functionality
</commit_message>
<xml_diff>
--- a/design/API.xlsx
+++ b/design/API.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920" firstSheet="10" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -604,18 +604,6 @@
   </si>
   <si>
     <t>{
-    orderID: 123456789,
-    rate: 5
-}</t>
-  </si>
-  <si>
-    <t>{
-    orderID: int,
-    rate: int
-}</t>
-  </si>
-  <si>
-    <t>{
     success: boolean,
     code: int,
     message: string,
@@ -1630,6 +1618,22 @@
   </si>
   <si>
     <t xml:space="preserve">get inprogress order list by sender id and receiver phone </t>
+  </si>
+  <si>
+    <t>{
+    orderID: int,
+    rate: int,
+   freedbackTitle: string,
+   feedbackContent: string,
+}</t>
+  </si>
+  <si>
+    <t>{
+    orderID: 123456789,
+    rate: 5,
+    feedbackTitle: 'fantastic order',
+    feedbackContent: 'this service is amazing'
+}</t>
   </si>
 </sst>
 </file>
@@ -2041,6 +2045,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2081,15 +2094,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2377,8 +2381,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2401,46 +2405,46 @@
         <v>36</v>
       </c>
       <c r="G1" s="54" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="57" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D2" s="37"/>
       <c r="G2" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="72"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="34" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D3" s="37"/>
       <c r="G3" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="7" t="s">
         <v>51</v>
       </c>
@@ -2449,93 +2453,93 @@
       </c>
       <c r="D4" s="37"/>
       <c r="G4" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D5" s="37"/>
       <c r="G5" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D6" s="37"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D7" s="37"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="72"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D8" s="37"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D9" s="37"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="73"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D11" s="36"/>
     </row>
@@ -2547,14 +2551,14 @@
         <v>53</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D12" s="37"/>
       <c r="G12" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2567,10 +2571,10 @@
       </c>
       <c r="D13" s="37"/>
       <c r="G13" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2591,7 +2595,7 @@
         <v>56</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D15" s="37"/>
       <c r="G15" s="4"/>
@@ -2600,10 +2604,10 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="52"/>
       <c r="B16" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D16" s="37"/>
       <c r="G16" s="4"/>
@@ -2612,10 +2616,10 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="52"/>
       <c r="B17" s="20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D17" s="37"/>
       <c r="G17" s="4"/>
@@ -2624,10 +2628,10 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="52"/>
       <c r="B18" s="20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D18" s="37"/>
       <c r="G18" s="4"/>
@@ -2636,10 +2640,10 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="52"/>
       <c r="B19" s="46" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D19" s="37"/>
       <c r="G19" s="4"/>
@@ -2648,10 +2652,10 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="56"/>
       <c r="B20" s="46" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D20" s="37"/>
       <c r="G20" s="4"/>
@@ -2669,10 +2673,10 @@
       </c>
       <c r="D21" s="37"/>
       <c r="G21" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2685,10 +2689,10 @@
       </c>
       <c r="D22" s="37"/>
       <c r="G22" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2701,10 +2705,10 @@
       </c>
       <c r="D23" s="37"/>
       <c r="G23" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2717,10 +2721,10 @@
       </c>
       <c r="D24" s="37"/>
       <c r="G24" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2733,10 +2737,10 @@
       </c>
       <c r="D25" s="37"/>
       <c r="G25" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2749,10 +2753,10 @@
       </c>
       <c r="D26" s="37"/>
       <c r="G26" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2765,10 +2769,10 @@
       </c>
       <c r="D27" s="37"/>
       <c r="G27" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2781,10 +2785,10 @@
       </c>
       <c r="D28" s="37"/>
       <c r="G28" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2810,42 +2814,42 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="45"/>
       <c r="B31" s="46" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D31" s="37"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="51" t="s">
+        <v>182</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>184</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>186</v>
       </c>
       <c r="D32" s="37"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="52"/>
       <c r="B33" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D33" s="37"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="52"/>
       <c r="B34" s="39" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D34" s="37"/>
     </row>
@@ -2864,19 +2868,19 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="38"/>
       <c r="C37" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="35"/>
       <c r="C38" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="37"/>
       <c r="C39" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2948,11 +2952,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="30" t="s">
         <v>47</v>
       </c>
@@ -2962,16 +2966,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -2983,21 +2987,21 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -3005,12 +3009,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="29" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -3021,7 +3025,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -3063,11 +3067,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="48" t="s">
         <v>47</v>
       </c>
@@ -3077,16 +3081,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
@@ -3098,21 +3102,21 @@
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3125,7 +3129,7 @@
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
       <c r="E5" s="49" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -3135,8 +3139,8 @@
       <c r="A6" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>238</v>
+      <c r="B6" s="71" t="s">
+        <v>236</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -3179,11 +3183,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3193,16 +3197,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3214,25 +3218,25 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="60" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3240,7 +3244,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="61" t="s">
         <v>82</v>
       </c>
       <c r="H5" s="3"/>
@@ -3248,7 +3252,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="5" t="s">
         <v>80</v>
       </c>
@@ -3256,13 +3260,13 @@
         <v>81</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="58"/>
+      <c r="E6" s="61"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="57"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -3270,7 +3274,7 @@
       <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="58"/>
+      <c r="E7" s="61"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -3323,11 +3327,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3342,11 +3346,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3358,9 +3362,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3437,11 +3441,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3456,11 +3460,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3472,9 +3476,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3490,7 +3494,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="60" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3498,7 +3502,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="61" t="s">
         <v>82</v>
       </c>
       <c r="H5" s="3"/>
@@ -3506,7 +3510,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="5" t="s">
         <v>80</v>
       </c>
@@ -3514,13 +3518,13 @@
         <v>89</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="58"/>
+      <c r="E6" s="61"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="57"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -3528,7 +3532,7 @@
       <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="58"/>
+      <c r="E7" s="61"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -3583,11 +3587,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -3597,16 +3601,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -3618,9 +3622,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3697,11 +3701,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3711,16 +3715,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3732,21 +3736,21 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3754,12 +3758,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="66" t="s">
-        <v>148</v>
+      <c r="E5" s="69" t="s">
+        <v>146</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -3771,10 +3775,10 @@
         <v>44</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="67"/>
+      <c r="E6" s="70"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -3783,8 +3787,8 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>155</v>
+      <c r="B7" s="71" t="s">
+        <v>153</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="53"/>
@@ -3826,11 +3830,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3840,16 +3844,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3861,21 +3865,21 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -3888,7 +3892,7 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -3898,8 +3902,8 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>166</v>
+      <c r="B6" s="71" t="s">
+        <v>164</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -3940,11 +3944,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3954,16 +3958,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -3975,21 +3979,21 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -4002,7 +4006,7 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -4012,8 +4016,8 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>178</v>
+      <c r="B6" s="71" t="s">
+        <v>176</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -4056,11 +4060,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="48" t="s">
         <v>47</v>
       </c>
@@ -4070,16 +4074,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
@@ -4091,21 +4095,21 @@
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4118,7 +4122,7 @@
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
       <c r="E5" s="49" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -4128,8 +4132,8 @@
       <c r="A6" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>238</v>
+      <c r="B6" s="71" t="s">
+        <v>236</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -4170,11 +4174,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -4184,16 +4188,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -4205,25 +4209,25 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="60" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -4231,7 +4235,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="61" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="3"/>
@@ -4239,7 +4243,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="5" t="s">
         <v>71</v>
       </c>
@@ -4247,13 +4251,13 @@
         <v>70</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="58"/>
+      <c r="E6" s="61"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="57"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
         <v>45</v>
@@ -4261,13 +4265,13 @@
       <c r="D7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="58"/>
+      <c r="E7" s="61"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="5"/>
       <c r="C8" s="7" t="s">
         <v>44</v>
@@ -4275,7 +4279,7 @@
       <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="58"/>
+      <c r="E8" s="61"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -4330,11 +4334,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="48" t="s">
         <v>47</v>
       </c>
@@ -4344,16 +4348,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
@@ -4365,21 +4369,21 @@
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4392,7 +4396,7 @@
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
       <c r="E5" s="49" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -4402,8 +4406,8 @@
       <c r="A6" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>244</v>
+      <c r="B6" s="71" t="s">
+        <v>242</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -4446,11 +4450,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4465,11 +4469,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4481,16 +4485,16 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -4507,7 +4511,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="69" t="s">
         <v>92</v>
       </c>
       <c r="H5" s="3"/>
@@ -4523,7 +4527,7 @@
         <v>73</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="67"/>
+      <c r="E6" s="70"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -4532,7 +4536,7 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="71" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="53"/>
@@ -4561,7 +4565,9 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4575,11 +4581,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4594,11 +4600,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4610,9 +4616,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -4647,7 +4653,7 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="71" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="53"/>
@@ -4691,11 +4697,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4710,11 +4716,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4726,16 +4732,16 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -4763,7 +4769,7 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="71" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="53"/>
@@ -4805,11 +4811,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4824,11 +4830,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4840,21 +4846,21 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4877,7 +4883,7 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="71" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="53"/>
@@ -4905,7 +4911,9 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4919,11 +4927,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4938,11 +4946,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -4954,21 +4962,21 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
+    </row>
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>97</v>
+        <v>251</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>96</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4991,7 +4999,7 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="71" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="53"/>
@@ -5033,11 +5041,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5052,11 +5060,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5068,21 +5076,21 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -5090,12 +5098,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="58" t="s">
-        <v>99</v>
+      <c r="E5" s="61" t="s">
+        <v>97</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -5110,7 +5118,7 @@
         <v>73</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="58"/>
+      <c r="E6" s="61"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5119,8 +5127,8 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>100</v>
+      <c r="B7" s="71" t="s">
+        <v>98</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="53"/>
@@ -5162,11 +5170,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5181,11 +5189,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5197,21 +5205,21 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5219,12 +5227,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -5234,7 +5242,7 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="71" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="53"/>
@@ -5278,11 +5286,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5297,11 +5305,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5313,16 +5321,16 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -5333,12 +5341,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -5348,7 +5356,7 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="71" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="53"/>
@@ -5390,11 +5398,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5409,11 +5417,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5425,21 +5433,21 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="405" x14ac:dyDescent="0.25">
@@ -5447,12 +5455,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -5462,7 +5470,7 @@
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="53"/>
@@ -5506,11 +5514,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="30" t="s">
         <v>47</v>
       </c>
@@ -5520,16 +5528,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -5541,21 +5549,21 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -5563,12 +5571,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -5606,7 +5614,9 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5620,11 +5630,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -5639,11 +5649,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -5655,21 +5665,21 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -5677,12 +5687,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="66" t="s">
-        <v>162</v>
+      <c r="E5" s="69" t="s">
+        <v>160</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -5694,10 +5704,10 @@
         <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="67"/>
+      <c r="E6" s="70"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5706,7 +5716,7 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="71" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="53"/>
@@ -5751,11 +5761,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="48" t="s">
         <v>47</v>
       </c>
@@ -5765,16 +5775,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
@@ -5786,21 +5796,21 @@
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -5808,12 +5818,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
-      <c r="E5" s="66" t="s">
-        <v>162</v>
+      <c r="E5" s="69" t="s">
+        <v>160</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -5825,10 +5835,10 @@
         <v>44</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D6" s="46"/>
-      <c r="E6" s="67"/>
+      <c r="E6" s="70"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5837,8 +5847,8 @@
       <c r="A7" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>252</v>
+      <c r="B7" s="71" t="s">
+        <v>250</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="53"/>
@@ -5880,11 +5890,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -5894,16 +5904,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -5915,47 +5925,47 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="72" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="66" t="s">
-        <v>193</v>
+      <c r="E5" s="69" t="s">
+        <v>191</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="70"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="67"/>
+      <c r="E6" s="70"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5964,8 +5974,8 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>192</v>
+      <c r="B7" s="71" t="s">
+        <v>190</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="53"/>
@@ -6008,11 +6018,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6022,16 +6032,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6043,21 +6053,21 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -6070,7 +6080,7 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -6080,8 +6090,8 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>197</v>
+      <c r="B6" s="71" t="s">
+        <v>195</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -6124,11 +6134,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="41" t="s">
         <v>47</v>
       </c>
@@ -6138,16 +6148,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -6159,21 +6169,21 @@
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
       <c r="E4" s="16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -6186,7 +6196,7 @@
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
       <c r="E5" s="42" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -6196,8 +6206,8 @@
       <c r="A6" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>231</v>
+      <c r="B6" s="71" t="s">
+        <v>229</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -6240,11 +6250,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
@@ -6259,11 +6269,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -6275,9 +6285,9 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -6289,31 +6299,31 @@
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="72" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="66" t="s">
-        <v>111</v>
+      <c r="E5" s="69" t="s">
+        <v>109</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="70"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="67"/>
+      <c r="E6" s="70"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -6322,7 +6332,7 @@
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="71" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="53"/>
@@ -6366,11 +6376,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -6385,11 +6395,11 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -6401,21 +6411,21 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -6428,7 +6438,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -6482,11 +6492,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
@@ -6496,16 +6506,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -6517,9 +6527,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -6543,7 +6553,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="61" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="3"/>
@@ -6559,7 +6569,7 @@
         <v>70</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="58"/>
+      <c r="E6" s="61"/>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -6570,7 +6580,7 @@
       <c r="D7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="58"/>
+      <c r="E7" s="61"/>
     </row>
     <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -6581,7 +6591,7 @@
       <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="58"/>
+      <c r="E8" s="61"/>
     </row>
     <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
@@ -6630,11 +6640,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6644,16 +6654,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6665,21 +6675,21 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -6687,12 +6697,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="66" t="s">
-        <v>148</v>
+      <c r="E5" s="69" t="s">
+        <v>146</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -6704,10 +6714,10 @@
         <v>44</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="67"/>
+      <c r="E6" s="70"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -6716,8 +6726,8 @@
       <c r="A7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>156</v>
+      <c r="B7" s="71" t="s">
+        <v>154</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="53"/>
@@ -6759,11 +6769,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6773,16 +6783,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6794,9 +6804,9 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -6817,7 +6827,7 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="25" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -6827,8 +6837,8 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>169</v>
+      <c r="B6" s="71" t="s">
+        <v>167</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -6869,11 +6879,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6883,16 +6893,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -6904,21 +6914,21 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -6931,7 +6941,7 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -6941,8 +6951,8 @@
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>176</v>
+      <c r="B6" s="71" t="s">
+        <v>174</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -6985,11 +6995,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
@@ -6999,16 +7009,16 @@
         <v>35</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="G2" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -7020,21 +7030,21 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -7058,7 +7068,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>

</xml_diff>

<commit_message>
add home screen in godelivery work app
</commit_message>
<xml_diff>
--- a/design/API.xlsx
+++ b/design/API.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920" firstSheet="10" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -2381,8 +2381,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3816,7 +3816,9 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4682,7 +4684,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G2" sqref="G2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4911,7 +4913,7 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -5027,7 +5029,9 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
finish user profile update
</commit_message>
<xml_diff>
--- a/design/API.xlsx
+++ b/design/API.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="920" firstSheet="15" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -1153,17 +1153,6 @@
   </si>
   <si>
     <t>{
-    sender: string,
-    receiver: string,
-    status: int,
-    beginCreatedAt: timestamp,
-    endCreatedAt: timestamp
-    pageNo: int,
-    pageSize: int,
-}</t>
-  </si>
-  <si>
-    <t>{
     "sender": "John Smith",
     "receiver": "Jane Doe",
     "status": 2,
@@ -1633,6 +1622,18 @@
     rate: 5,
     feedbackTitle: 'fantastic order',
     feedbackContent: 'this service is amazing'
+}</t>
+  </si>
+  <si>
+    <t>{
+    sender: string,
+    receiver: string,
+    deliverymanID: string,
+    status: int,
+    beginCreatedAt: timestamp,
+    endCreatedAt: timestamp
+    pageNo: int,
+    pageSize: int,
 }</t>
   </si>
 </sst>
@@ -2381,8 +2382,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2433,7 +2434,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3" s="37"/>
       <c r="G3" s="4" t="s">
@@ -2465,7 +2466,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D5" s="37"/>
       <c r="G5" s="4" t="s">
@@ -2514,10 +2515,10 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="58"/>
       <c r="B9" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D9" s="37"/>
       <c r="G9" s="4"/>
@@ -2526,20 +2527,20 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="58"/>
       <c r="B10" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>197</v>
       </c>
       <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="59"/>
       <c r="B11" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D11" s="36"/>
     </row>
@@ -2551,7 +2552,7 @@
         <v>53</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D12" s="37"/>
       <c r="G12" s="4" t="s">
@@ -2595,7 +2596,7 @@
         <v>56</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D15" s="37"/>
       <c r="G15" s="4"/>
@@ -2640,10 +2641,10 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="52"/>
       <c r="B19" s="46" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>232</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>233</v>
       </c>
       <c r="D19" s="37"/>
       <c r="G19" s="4"/>
@@ -2652,10 +2653,10 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="56"/>
       <c r="B20" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>237</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>238</v>
       </c>
       <c r="D20" s="37"/>
       <c r="G20" s="4"/>
@@ -2814,42 +2815,42 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="45"/>
       <c r="B31" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>247</v>
       </c>
       <c r="D31" s="37"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="51" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="C32" s="17" t="s">
         <v>183</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>184</v>
       </c>
       <c r="D32" s="37"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="52"/>
       <c r="B33" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>185</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>186</v>
       </c>
       <c r="D33" s="37"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="52"/>
       <c r="B34" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>227</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>228</v>
       </c>
       <c r="D34" s="37"/>
     </row>
@@ -2868,19 +2869,19 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="38"/>
       <c r="C37" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="35"/>
       <c r="C38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="37"/>
       <c r="C39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2966,7 +2967,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2996,12 +2997,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -3009,12 +3010,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -3025,7 +3026,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -3081,7 +3082,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -3111,12 +3112,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3140,7 +3141,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -3197,7 +3198,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3601,7 +3602,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -4076,7 +4077,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -4106,12 +4107,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4135,7 +4136,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -4350,7 +4351,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -4380,12 +4381,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4398,7 +4399,7 @@
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
       <c r="E5" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -4409,7 +4410,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -4496,7 +4497,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -4743,7 +4744,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -4857,12 +4858,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4973,12 +4974,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -5089,12 +5090,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -5334,7 +5335,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -5532,7 +5533,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -5562,12 +5563,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -5575,12 +5576,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -5673,17 +5674,17 @@
       <c r="H3" s="67"/>
       <c r="I3" s="68"/>
     </row>
-    <row r="4" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>178</v>
+        <v>252</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -5779,7 +5780,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -5809,12 +5810,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -5852,7 +5853,7 @@
         <v>43</v>
       </c>
       <c r="B7" s="71" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="53"/>
@@ -5880,7 +5881,9 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5908,7 +5911,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -5938,7 +5941,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -5949,12 +5952,12 @@
         <v>33</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -5963,10 +5966,10 @@
     <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="73"/>
       <c r="B6" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>188</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>189</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="70"/>
@@ -5979,7 +5982,7 @@
         <v>43</v>
       </c>
       <c r="B7" s="71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="53"/>
@@ -6036,7 +6039,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -6066,12 +6069,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -6084,7 +6087,7 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -6095,7 +6098,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -6152,7 +6155,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
@@ -6182,12 +6185,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
       <c r="E4" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -6200,7 +6203,7 @@
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
       <c r="E5" s="42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -6211,7 +6214,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="71" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -6424,12 +6427,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -6442,7 +6445,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -6510,7 +6513,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -6831,7 +6834,7 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="12"/>
@@ -7013,7 +7016,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -7043,12 +7046,12 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -7072,7 +7075,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>

</xml_diff>